<commit_message>
modiefid HW.xlsx add myscript
</commit_message>
<xml_diff>
--- a/HW.xlsx
+++ b/HW.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\курсы\рисунки_плакаты\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Kursy_copy\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A5BB18-8AE8-4E69-A8B3-1050DE427049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1C0F17-0D89-473F-AF3D-2FC2AD92CCEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="классификация тестирования" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист4" sheetId="4" r:id="rId2"/>
-    <sheet name="цели" sheetId="2" r:id="rId3"/>
-    <sheet name="Принципы" sheetId="3" r:id="rId4"/>
+    <sheet name="Git.HW 1" sheetId="4" r:id="rId2"/>
+    <sheet name="цели тестир" sheetId="2" r:id="rId3"/>
+    <sheet name="Принципы тестир" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1107,12 +1107,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1840,250 +1848,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2092,73 +1989,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2167,8 +2013,170 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2466,1548 +2474,1601 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="3.28515625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="9"/>
-    <col min="13" max="13" width="4" style="9" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="15" width="16.140625" style="9" customWidth="1"/>
-    <col min="16" max="16" width="5" style="9" customWidth="1"/>
-    <col min="17" max="17" width="3.42578125" style="9" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" style="9" customWidth="1"/>
-    <col min="19" max="19" width="5" style="9" customWidth="1"/>
-    <col min="20" max="20" width="4" style="9" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" style="9" customWidth="1"/>
-    <col min="22" max="23" width="9.140625" style="9"/>
-    <col min="24" max="24" width="16.140625" style="9" customWidth="1"/>
-    <col min="25" max="25" width="5" style="9" customWidth="1"/>
-    <col min="26" max="26" width="3.85546875" style="9" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" style="9" customWidth="1"/>
-    <col min="28" max="28" width="5" style="9" customWidth="1"/>
-    <col min="29" max="29" width="3.140625" style="9" customWidth="1"/>
-    <col min="30" max="30" width="16.140625" style="9" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="2.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
+    <col min="13" max="13" width="4" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="16.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="5" style="3" customWidth="1"/>
+    <col min="17" max="17" width="3.42578125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="5" style="3" customWidth="1"/>
+    <col min="20" max="20" width="4" style="3" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" style="3" customWidth="1"/>
+    <col min="22" max="23" width="9.140625" style="3"/>
+    <col min="24" max="24" width="16.140625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="5" style="3" customWidth="1"/>
+    <col min="26" max="26" width="3.85546875" style="3" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="5" style="3" customWidth="1"/>
+    <col min="29" max="29" width="3.140625" style="3" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" style="3" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="11" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
     </row>
     <row r="2" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="N2" s="15"/>
-      <c r="V2" s="13"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="V2" s="6"/>
     </row>
     <row r="3" spans="1:30" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="22" t="s">
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="93"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="25" t="s">
+      <c r="P3" s="110"/>
+      <c r="Q3" s="110"/>
+      <c r="R3" s="110"/>
+      <c r="S3" s="110"/>
+      <c r="T3" s="110"/>
+      <c r="U3" s="111"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="27"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
+      <c r="AB3" s="104"/>
+      <c r="AC3" s="104"/>
+      <c r="AD3" s="105"/>
     </row>
     <row r="4" spans="1:30" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="G4" s="28"/>
-      <c r="K4" s="29"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="16"/>
-      <c r="U4" s="28"/>
-      <c r="W4" s="30"/>
-      <c r="Z4" s="28"/>
-      <c r="AD4" s="28"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="G4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="9"/>
+      <c r="U4" s="12"/>
+      <c r="W4" s="14"/>
+      <c r="Z4" s="12"/>
+      <c r="AD4" s="12"/>
     </row>
     <row r="5" spans="1:30" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="E5" s="33" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="E5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35"/>
-      <c r="J5" s="33" t="s">
+      <c r="F5" s="59"/>
+      <c r="G5" s="60"/>
+      <c r="J5" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="29" t="s">
+      <c r="K5" s="60"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="R5" s="29" t="s">
+      <c r="P5" s="9"/>
+      <c r="R5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="16"/>
-      <c r="U5" s="29" t="s">
+      <c r="S5" s="9"/>
+      <c r="U5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="W5" s="36"/>
-      <c r="X5" s="33" t="s">
+      <c r="W5" s="17"/>
+      <c r="X5" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="35"/>
-      <c r="AC5" s="33" t="s">
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="60"/>
+      <c r="AC5" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="AD5" s="35"/>
+      <c r="AD5" s="60"/>
     </row>
     <row r="6" spans="1:30" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="N6" s="30"/>
-      <c r="W6" s="30"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="N6" s="14"/>
+      <c r="W6" s="14"/>
     </row>
     <row r="7" spans="1:30" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="18" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="6" t="s">
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="93"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="8"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="25" t="s">
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
+      <c r="S7" s="101"/>
+      <c r="T7" s="101"/>
+      <c r="U7" s="102"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="27"/>
+      <c r="Y7" s="104"/>
+      <c r="Z7" s="104"/>
+      <c r="AA7" s="104"/>
+      <c r="AB7" s="104"/>
+      <c r="AC7" s="104"/>
+      <c r="AD7" s="105"/>
     </row>
     <row r="8" spans="1:30" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="16"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="30"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="16"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="16"/>
-      <c r="U8" s="28"/>
-      <c r="W8" s="30"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="16"/>
-      <c r="AD8" s="42"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="9"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="14"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="9"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="9"/>
+      <c r="U8" s="12"/>
+      <c r="W8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="9"/>
+      <c r="AD8" s="20"/>
     </row>
     <row r="9" spans="1:30" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="45" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="29" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="29" t="s">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="36"/>
-      <c r="O9" s="29" t="s">
+      <c r="N9" s="17"/>
+      <c r="O9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="16"/>
-      <c r="R9" s="29" t="s">
+      <c r="P9" s="9"/>
+      <c r="R9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S9" s="16"/>
-      <c r="U9" s="29" t="s">
+      <c r="S9" s="9"/>
+      <c r="U9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="V9" s="44"/>
-      <c r="X9" s="29" t="s">
+      <c r="V9" s="22"/>
+      <c r="X9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="45" t="s">
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="AB9" s="16"/>
-      <c r="AD9" s="29" t="s">
+      <c r="AB9" s="9"/>
+      <c r="AD9" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="N10" s="30"/>
-      <c r="W10" s="30"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="N10" s="14"/>
+      <c r="W10" s="14"/>
     </row>
     <row r="11" spans="1:30" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="18" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="38" t="s">
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="40"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="47" t="s">
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="108"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="48"/>
-      <c r="AA11" s="48"/>
-      <c r="AB11" s="48"/>
-      <c r="AC11" s="48"/>
-      <c r="AD11" s="49"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="89"/>
+      <c r="AA11" s="89"/>
+      <c r="AB11" s="89"/>
+      <c r="AC11" s="89"/>
+      <c r="AD11" s="90"/>
     </row>
     <row r="12" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="28"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="16"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="16"/>
-      <c r="U12" s="28"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="42"/>
-      <c r="AB12" s="16"/>
-      <c r="AD12" s="42"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="12"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="9"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="9"/>
+      <c r="U12" s="12"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="9"/>
+      <c r="AD12" s="20"/>
     </row>
     <row r="13" spans="1:30" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="29" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="29" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="29" t="s">
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="O13" s="29" t="s">
+      <c r="O13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="29" t="s">
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="S13" s="16"/>
-      <c r="U13" s="29" t="s">
+      <c r="S13" s="9"/>
+      <c r="U13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X13" s="29" t="s">
+      <c r="X13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="Y13" s="16"/>
-      <c r="AA13" s="29" t="s">
+      <c r="Y13" s="9"/>
+      <c r="AA13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AB13" s="16"/>
-      <c r="AD13" s="29" t="s">
+      <c r="AB13" s="9"/>
+      <c r="AD13" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+      <c r="A14" s="5"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:30" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="E15" s="52"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="10"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="E15" s="27"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:30" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="53" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="55"/>
-      <c r="P16" s="13"/>
-      <c r="R16" s="56" t="s">
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="95"/>
+      <c r="L16" s="95"/>
+      <c r="M16" s="95"/>
+      <c r="N16" s="96"/>
+      <c r="P16" s="6"/>
+      <c r="R16" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
-      <c r="U16" s="57"/>
-      <c r="V16" s="57"/>
-      <c r="W16" s="57"/>
-      <c r="X16" s="58"/>
+      <c r="S16" s="98"/>
+      <c r="T16" s="98"/>
+      <c r="U16" s="98"/>
+      <c r="V16" s="98"/>
+      <c r="W16" s="98"/>
+      <c r="X16" s="99"/>
     </row>
     <row r="17" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="16"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="P17" s="12"/>
-      <c r="R17" s="31"/>
-      <c r="T17" s="59"/>
-      <c r="X17" s="59"/>
-      <c r="Y17" s="50"/>
-      <c r="AA17" s="60"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="9"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="P17" s="5"/>
+      <c r="R17" s="15"/>
+      <c r="T17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="25"/>
+      <c r="AA17" s="29"/>
     </row>
     <row r="18" spans="1:31" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="81" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="82"/>
-      <c r="F18" s="12"/>
-      <c r="H18" s="29" t="s">
+      <c r="E18" s="79"/>
+      <c r="F18" s="5"/>
+      <c r="H18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="K18" s="29" t="s">
+      <c r="I18" s="5"/>
+      <c r="K18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="P18" s="12"/>
-      <c r="R18" s="29" t="s">
+      <c r="P18" s="5"/>
+      <c r="R18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T18" s="12"/>
-      <c r="U18" s="62" t="s">
+      <c r="T18" s="5"/>
+      <c r="U18" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="X18" s="12"/>
-      <c r="Z18" s="63" t="s">
+      <c r="X18" s="5"/>
+      <c r="Z18" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="AA18" s="64"/>
-      <c r="AB18" s="64"/>
-      <c r="AC18" s="64"/>
-      <c r="AD18" s="64"/>
-      <c r="AE18" s="65"/>
+      <c r="AA18" s="85"/>
+      <c r="AB18" s="85"/>
+      <c r="AC18" s="85"/>
+      <c r="AD18" s="85"/>
+      <c r="AE18" s="86"/>
     </row>
     <row r="19" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="16"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="14"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="14"/>
-      <c r="P19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="43"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="9"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="7"/>
+      <c r="P19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="21"/>
     </row>
     <row r="20" spans="1:31" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="43"/>
-      <c r="F20" s="12"/>
-      <c r="H20" s="29" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="21"/>
+      <c r="F20" s="5"/>
+      <c r="H20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="63" t="s">
+      <c r="I20" s="5"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="S20" s="64"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="65"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="43"/>
-      <c r="Z20" s="17"/>
-      <c r="AA20" s="33" t="s">
+      <c r="S20" s="85"/>
+      <c r="T20" s="85"/>
+      <c r="U20" s="86"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="34"/>
-      <c r="AD20" s="35"/>
+      <c r="AB20" s="59"/>
+      <c r="AC20" s="59"/>
+      <c r="AD20" s="60"/>
     </row>
     <row r="21" spans="1:31" ht="43.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="50"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="66"/>
-      <c r="I21" s="12"/>
-      <c r="K21" s="29" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="25"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="32"/>
+      <c r="I21" s="5"/>
+      <c r="K21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="P21" s="12"/>
-      <c r="R21" s="59"/>
-      <c r="T21" s="59"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="43"/>
+      <c r="P21" s="5"/>
+      <c r="R21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="21"/>
     </row>
     <row r="22" spans="1:31" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="21"/>
       <c r="E22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="14"/>
-      <c r="P22" s="12"/>
-      <c r="R22" s="33" t="s">
+      <c r="F22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="7"/>
+      <c r="P22" s="5"/>
+      <c r="R22" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="S22" s="35"/>
-      <c r="U22" s="33" t="s">
+      <c r="S22" s="60"/>
+      <c r="U22" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="V22" s="35"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="43"/>
-      <c r="AA22" s="33" t="s">
+      <c r="V22" s="60"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="21"/>
+      <c r="AA22" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="AB22" s="34"/>
-      <c r="AC22" s="34"/>
-      <c r="AD22" s="35"/>
+      <c r="AB22" s="59"/>
+      <c r="AC22" s="59"/>
+      <c r="AD22" s="60"/>
     </row>
     <row r="23" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="43"/>
-      <c r="F23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="K23" s="29" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="21"/>
+      <c r="F23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="K23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="P23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="14"/>
+      <c r="P23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="21"/>
+      <c r="Z23" s="7"/>
     </row>
     <row r="24" spans="1:31" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="29" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="14"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="63" t="s">
+      <c r="F24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="7"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="65"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="17"/>
-      <c r="AA24" s="33" t="s">
+      <c r="S24" s="85"/>
+      <c r="T24" s="85"/>
+      <c r="U24" s="86"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="AB24" s="34"/>
-      <c r="AC24" s="34"/>
-      <c r="AD24" s="35"/>
+      <c r="AB24" s="59"/>
+      <c r="AC24" s="59"/>
+      <c r="AD24" s="60"/>
     </row>
     <row r="25" spans="1:31" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="K25" s="29" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="K25" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="M25" s="21"/>
-      <c r="N25" s="63" t="s">
+      <c r="M25" s="11"/>
+      <c r="N25" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="O25" s="65"/>
-      <c r="P25" s="67"/>
-      <c r="R25" s="59"/>
-      <c r="U25" s="83"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="43"/>
-      <c r="Z25" s="14"/>
+      <c r="O25" s="86"/>
+      <c r="P25" s="33"/>
+      <c r="R25" s="28"/>
+      <c r="U25" s="46"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="7"/>
     </row>
     <row r="26" spans="1:31" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="J26" s="66"/>
-      <c r="L26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="R26" s="33" t="s">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="J26" s="32"/>
+      <c r="L26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="R26" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="S26" s="35"/>
-      <c r="U26" s="33" t="s">
+      <c r="S26" s="60"/>
+      <c r="U26" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="V26" s="35"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="43"/>
-      <c r="AA26" s="33" t="s">
+      <c r="V26" s="60"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="21"/>
+      <c r="AA26" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="AB26" s="34"/>
-      <c r="AC26" s="34"/>
-      <c r="AD26" s="35"/>
+      <c r="AB26" s="59"/>
+      <c r="AC26" s="59"/>
+      <c r="AD26" s="60"/>
     </row>
     <row r="27" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="30"/>
-      <c r="P27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Z27" s="66"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="14"/>
+      <c r="P27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Z27" s="32"/>
     </row>
     <row r="28" spans="1:31" ht="44.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="29" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="12"/>
-      <c r="H28" s="29" t="s">
+      <c r="F28" s="5"/>
+      <c r="H28" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="16"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="33" t="s">
+      <c r="K28" s="9"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="O28" s="35"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="63" t="s">
+      <c r="O28" s="60"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="S28" s="64"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="64"/>
-      <c r="W28" s="65"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="14"/>
-      <c r="Z28" s="68"/>
-      <c r="AA28" s="63" t="s">
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="85"/>
+      <c r="V28" s="85"/>
+      <c r="W28" s="86"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="AB28" s="64"/>
-      <c r="AC28" s="64"/>
-      <c r="AD28" s="65"/>
+      <c r="AB28" s="85"/>
+      <c r="AC28" s="85"/>
+      <c r="AD28" s="86"/>
     </row>
     <row r="29" spans="1:31" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="14"/>
-      <c r="L29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="S29" s="59"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="43"/>
-      <c r="Z29" s="66"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="7"/>
+      <c r="L29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="S29" s="28"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="21"/>
+      <c r="Z29" s="32"/>
     </row>
     <row r="30" spans="1:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="S30" s="12"/>
-      <c r="X30" s="12"/>
-      <c r="Y30" s="43"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="21"/>
     </row>
     <row r="31" spans="1:31" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="29" t="s">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="29" t="s">
+      <c r="F31" s="5"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="12"/>
-      <c r="M31" s="66"/>
-      <c r="N31" s="33" t="s">
+      <c r="L31" s="5"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="O31" s="35"/>
-      <c r="P31" s="12"/>
-      <c r="S31" s="12"/>
-      <c r="U31" s="33" t="s">
+      <c r="O31" s="60"/>
+      <c r="P31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="U31" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="V31" s="34"/>
-      <c r="W31" s="35"/>
-      <c r="X31" s="12"/>
-      <c r="Y31" s="43"/>
-      <c r="AA31" s="33" t="s">
+      <c r="V31" s="59"/>
+      <c r="W31" s="60"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="21"/>
+      <c r="AA31" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="AB31" s="34"/>
-      <c r="AC31" s="34"/>
-      <c r="AD31" s="35"/>
+      <c r="AB31" s="59"/>
+      <c r="AC31" s="59"/>
+      <c r="AD31" s="60"/>
     </row>
     <row r="32" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="S32" s="12"/>
-      <c r="T32" s="14"/>
-      <c r="X32" s="12"/>
-      <c r="Y32" s="43"/>
-      <c r="Z32" s="14"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="7"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="7"/>
     </row>
     <row r="33" spans="1:30" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="29" t="s">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="62" t="s">
+      <c r="F33" s="5"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="L33" s="12"/>
-      <c r="N33" s="33" t="s">
+      <c r="L33" s="5"/>
+      <c r="N33" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="O33" s="35"/>
-      <c r="P33" s="12"/>
-      <c r="S33" s="12"/>
-      <c r="U33" s="33" t="s">
+      <c r="O33" s="60"/>
+      <c r="P33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="U33" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="V33" s="34"/>
-      <c r="W33" s="35"/>
-      <c r="X33" s="12"/>
-      <c r="Y33" s="43"/>
-      <c r="Z33" s="17"/>
-      <c r="AA33" s="33" t="s">
+      <c r="V33" s="59"/>
+      <c r="W33" s="60"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="21"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="AB33" s="34"/>
-      <c r="AC33" s="34"/>
-      <c r="AD33" s="35"/>
+      <c r="AB33" s="59"/>
+      <c r="AC33" s="59"/>
+      <c r="AD33" s="60"/>
     </row>
     <row r="34" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="14"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="14"/>
-      <c r="M34" s="66"/>
-      <c r="P34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="14"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="50"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="7"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="7"/>
+      <c r="M34" s="32"/>
+      <c r="P34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="7"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="25"/>
     </row>
     <row r="35" spans="1:30" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="E35" s="29" t="s">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="E35" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="29" t="s">
+      <c r="F35" s="5"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="P35" s="12"/>
-      <c r="S35" s="12"/>
-      <c r="U35" s="33" t="s">
+      <c r="P35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="U35" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="V35" s="34"/>
-      <c r="W35" s="35"/>
-      <c r="X35" s="16"/>
-      <c r="Y35" s="66"/>
-      <c r="Z35" s="68"/>
-      <c r="AA35" s="63" t="s">
+      <c r="V35" s="59"/>
+      <c r="W35" s="60"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="32"/>
+      <c r="Z35" s="34"/>
+      <c r="AA35" s="84" t="s">
         <v>105</v>
       </c>
-      <c r="AB35" s="64"/>
-      <c r="AC35" s="64"/>
-      <c r="AD35" s="65"/>
+      <c r="AB35" s="85"/>
+      <c r="AC35" s="85"/>
+      <c r="AD35" s="86"/>
     </row>
     <row r="36" spans="1:30" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="66"/>
-      <c r="F36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="S36" s="12"/>
-      <c r="T36" s="14"/>
-      <c r="X36" s="16"/>
-      <c r="Y36" s="16"/>
-      <c r="Z36" s="12"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="32"/>
+      <c r="F36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="7"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
+      <c r="Z36" s="5"/>
     </row>
     <row r="37" spans="1:30" ht="41.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="29" t="s">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="29" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K37" s="12"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="63" t="s">
+      <c r="K37" s="5"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="N37" s="64"/>
-      <c r="O37" s="65"/>
-      <c r="P37" s="67"/>
-      <c r="S37" s="12"/>
-      <c r="U37" s="33" t="s">
+      <c r="N37" s="85"/>
+      <c r="O37" s="86"/>
+      <c r="P37" s="33"/>
+      <c r="S37" s="5"/>
+      <c r="U37" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="V37" s="34"/>
-      <c r="W37" s="35"/>
-      <c r="Z37" s="12"/>
-      <c r="AA37" s="17"/>
-      <c r="AB37" s="33" t="s">
+      <c r="V37" s="59"/>
+      <c r="W37" s="60"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="10"/>
+      <c r="AB37" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="AC37" s="34"/>
-      <c r="AD37" s="35"/>
+      <c r="AC37" s="59"/>
+      <c r="AD37" s="60"/>
     </row>
     <row r="38" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="P38" s="12"/>
-      <c r="S38" s="12"/>
-      <c r="T38" s="66"/>
-      <c r="Z38" s="12"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="32"/>
+      <c r="Z38" s="5"/>
     </row>
     <row r="39" spans="1:30" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="29" t="s">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F39" s="12"/>
-      <c r="H39" s="61" t="s">
+      <c r="F39" s="5"/>
+      <c r="H39" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="I39" s="69"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="33" t="s">
+      <c r="I39" s="35"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="O39" s="35"/>
-      <c r="P39" s="12"/>
-      <c r="S39" s="12"/>
-      <c r="T39" s="43"/>
-      <c r="U39" s="70" t="s">
+      <c r="O39" s="60"/>
+      <c r="P39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="V39" s="34"/>
-      <c r="W39" s="35"/>
-      <c r="Z39" s="12"/>
-      <c r="AA39" s="17"/>
-      <c r="AB39" s="33" t="s">
+      <c r="V39" s="59"/>
+      <c r="W39" s="60"/>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="10"/>
+      <c r="AB39" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="AC39" s="34"/>
-      <c r="AD39" s="35"/>
+      <c r="AC39" s="59"/>
+      <c r="AD39" s="60"/>
     </row>
     <row r="40" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="15"/>
-      <c r="G40" s="66"/>
-      <c r="I40" s="13"/>
-      <c r="K40" s="12"/>
-      <c r="P40" s="12"/>
-      <c r="T40" s="71"/>
-      <c r="Z40" s="12"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="8"/>
+      <c r="G40" s="32"/>
+      <c r="I40" s="6"/>
+      <c r="K40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="T40" s="36"/>
+      <c r="Z40" s="5"/>
     </row>
     <row r="41" spans="1:30" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="61" t="s">
+      <c r="A41" s="5"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="H41" s="29" t="s">
+      <c r="H41" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="50"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="33" t="s">
+      <c r="I41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="O41" s="35"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="50"/>
-      <c r="R41" s="63" t="s">
+      <c r="O41" s="60"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="64"/>
-      <c r="T41" s="64"/>
-      <c r="U41" s="64"/>
-      <c r="V41" s="64"/>
-      <c r="W41" s="65"/>
-      <c r="Z41" s="12"/>
-      <c r="AA41" s="17"/>
-      <c r="AB41" s="33" t="s">
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="85"/>
+      <c r="V41" s="85"/>
+      <c r="W41" s="86"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="AC41" s="34"/>
-      <c r="AD41" s="35"/>
+      <c r="AC41" s="59"/>
+      <c r="AD41" s="60"/>
     </row>
     <row r="42" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="D42" s="14"/>
-      <c r="I42" s="13"/>
-      <c r="K42" s="12"/>
-      <c r="P42" s="16"/>
-      <c r="R42" s="16"/>
-      <c r="S42" s="59"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
-      <c r="V42" s="16"/>
-      <c r="Z42" s="12"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="D42" s="7"/>
+      <c r="I42" s="6"/>
+      <c r="K42" s="5"/>
+      <c r="P42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
+      <c r="V42" s="9"/>
+      <c r="Z42" s="5"/>
     </row>
     <row r="43" spans="1:30" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="29" t="s">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H43" s="29" t="s">
+      <c r="H43" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="50"/>
-      <c r="M43" s="37"/>
-      <c r="N43" s="33" t="s">
+      <c r="I43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="O43" s="35"/>
-      <c r="P43" s="16"/>
-      <c r="S43" s="12"/>
-      <c r="T43" s="17"/>
-      <c r="U43" s="33" t="s">
+      <c r="O43" s="60"/>
+      <c r="P43" s="9"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="V43" s="34"/>
-      <c r="W43" s="35"/>
-      <c r="Z43" s="12"/>
-      <c r="AB43" s="33" t="s">
+      <c r="V43" s="59"/>
+      <c r="W43" s="60"/>
+      <c r="Z43" s="5"/>
+      <c r="AB43" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="AC43" s="34"/>
-      <c r="AD43" s="35"/>
+      <c r="AC43" s="59"/>
+      <c r="AD43" s="60"/>
     </row>
     <row r="44" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="D44" s="14"/>
-      <c r="I44" s="13"/>
-      <c r="K44" s="12"/>
-      <c r="O44" s="73"/>
-      <c r="P44" s="16"/>
-      <c r="R44" s="16"/>
-      <c r="S44" s="12"/>
-      <c r="T44" s="16"/>
-      <c r="U44" s="16"/>
-      <c r="V44" s="16"/>
-      <c r="Z44" s="12"/>
-      <c r="AA44" s="14"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="D44" s="7"/>
+      <c r="I44" s="6"/>
+      <c r="K44" s="5"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="7"/>
     </row>
     <row r="45" spans="1:30" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="29" t="s">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H45" s="29" t="s">
+      <c r="H45" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="I45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="50"/>
-      <c r="M45" s="37"/>
-      <c r="N45" s="33" t="s">
+      <c r="I45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="25"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="O45" s="35"/>
-      <c r="P45" s="16"/>
-      <c r="S45" s="12"/>
-      <c r="U45" s="33" t="s">
+      <c r="O45" s="60"/>
+      <c r="P45" s="9"/>
+      <c r="S45" s="5"/>
+      <c r="U45" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="V45" s="34"/>
-      <c r="W45" s="35"/>
-      <c r="Z45" s="12"/>
-      <c r="AA45" s="17"/>
-      <c r="AB45" s="33" t="s">
+      <c r="V45" s="59"/>
+      <c r="W45" s="60"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="10"/>
+      <c r="AB45" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="AC45" s="34"/>
-      <c r="AD45" s="35"/>
+      <c r="AC45" s="59"/>
+      <c r="AD45" s="60"/>
     </row>
     <row r="46" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="I46" s="13"/>
-      <c r="K46" s="12"/>
-      <c r="P46" s="16"/>
-      <c r="R46" s="16"/>
-      <c r="S46" s="12"/>
-      <c r="T46" s="14"/>
-      <c r="U46" s="16"/>
-      <c r="V46" s="16"/>
-      <c r="Z46" s="12"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="I46" s="6"/>
+      <c r="K46" s="5"/>
+      <c r="P46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="9"/>
+      <c r="V46" s="9"/>
+      <c r="Z46" s="5"/>
     </row>
     <row r="47" spans="1:30" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="29" t="s">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H47" s="29" t="s">
+      <c r="H47" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I47" s="74"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="50"/>
-      <c r="M47" s="37"/>
-      <c r="N47" s="33" t="s">
+      <c r="I47" s="39"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="O47" s="35"/>
-      <c r="P47" s="16"/>
-      <c r="S47" s="12"/>
-      <c r="T47" s="17"/>
-      <c r="U47" s="33" t="s">
+      <c r="O47" s="60"/>
+      <c r="P47" s="9"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="V47" s="34"/>
-      <c r="W47" s="35"/>
-      <c r="Z47" s="12"/>
-      <c r="AA47" s="17"/>
-      <c r="AB47" s="33" t="s">
+      <c r="V47" s="59"/>
+      <c r="W47" s="60"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="10"/>
+      <c r="AB47" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="AC47" s="34"/>
-      <c r="AD47" s="35"/>
+      <c r="AC47" s="59"/>
+      <c r="AD47" s="60"/>
     </row>
     <row r="48" spans="1:30" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="P48" s="16"/>
-      <c r="R48" s="16"/>
-      <c r="S48" s="12"/>
-      <c r="T48" s="16"/>
-      <c r="U48" s="16"/>
-      <c r="V48" s="16"/>
-      <c r="Z48" s="12"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="P48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="Z48" s="5"/>
     </row>
     <row r="49" spans="1:31" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="29" t="s">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H49" s="29" t="s">
+      <c r="H49" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I49" s="74"/>
-      <c r="K49" s="75"/>
-      <c r="L49" s="50"/>
-      <c r="N49" s="33" t="s">
+      <c r="I49" s="39"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="25"/>
+      <c r="N49" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="O49" s="35"/>
-      <c r="P49" s="16"/>
-      <c r="S49" s="12"/>
-      <c r="T49" s="17"/>
-      <c r="U49" s="33" t="s">
+      <c r="O49" s="60"/>
+      <c r="P49" s="9"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="V49" s="34"/>
-      <c r="W49" s="35"/>
-      <c r="Z49" s="12"/>
-      <c r="AB49" s="3" t="s">
+      <c r="V49" s="59"/>
+      <c r="W49" s="60"/>
+      <c r="Z49" s="5"/>
+      <c r="AB49" s="80" t="s">
         <v>110</v>
       </c>
-      <c r="AC49" s="4"/>
-      <c r="AD49" s="5"/>
+      <c r="AC49" s="81"/>
+      <c r="AD49" s="82"/>
     </row>
     <row r="50" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="14"/>
-      <c r="K50" s="12"/>
-      <c r="M50" s="66"/>
-      <c r="P50" s="16"/>
-      <c r="U50" s="16"/>
-      <c r="Z50" s="12"/>
-      <c r="AA50" s="14"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="7"/>
+      <c r="K50" s="5"/>
+      <c r="M50" s="32"/>
+      <c r="P50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="7"/>
     </row>
     <row r="51" spans="1:31" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="76"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="78" t="s">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="F51" s="79"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="50"/>
-      <c r="N51" s="33" t="s">
+      <c r="F51" s="44"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="25"/>
+      <c r="N51" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="O51" s="35"/>
-      <c r="P51" s="80"/>
-      <c r="Z51" s="12"/>
-      <c r="AA51" s="17"/>
-      <c r="AB51" s="33" t="s">
+      <c r="O51" s="60"/>
+      <c r="P51" s="45"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="10"/>
+      <c r="AB51" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="AC51" s="34"/>
-      <c r="AD51" s="35"/>
+      <c r="AC51" s="59"/>
+      <c r="AD51" s="60"/>
     </row>
     <row r="52" spans="1:31" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="100"/>
-      <c r="M52" s="66"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="54"/>
+      <c r="M52" s="32"/>
     </row>
     <row r="53" spans="1:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="99"/>
+      <c r="A53" s="5"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="53"/>
     </row>
     <row r="54" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="66"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="33" t="s">
+      <c r="B54" s="32"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
-      <c r="O54" s="34"/>
-      <c r="P54" s="34"/>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="34"/>
-      <c r="S54" s="34"/>
-      <c r="T54" s="34"/>
-      <c r="U54" s="34"/>
-      <c r="V54" s="34"/>
-      <c r="W54" s="35"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
+      <c r="J54" s="59"/>
+      <c r="K54" s="59"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="59"/>
+      <c r="Q54" s="59"/>
+      <c r="R54" s="59"/>
+      <c r="S54" s="59"/>
+      <c r="T54" s="59"/>
+      <c r="U54" s="59"/>
+      <c r="V54" s="59"/>
+      <c r="W54" s="60"/>
     </row>
     <row r="55" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="12"/>
-      <c r="E55" s="31"/>
-      <c r="W55" s="28"/>
+      <c r="B55" s="5"/>
+      <c r="E55" s="15"/>
+      <c r="W55" s="12"/>
     </row>
     <row r="56" spans="1:31" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="12"/>
-      <c r="D56" s="33" t="s">
+      <c r="B56" s="5"/>
+      <c r="D56" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="35"/>
-      <c r="L56" s="33" t="s">
+      <c r="E56" s="59"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59"/>
+      <c r="H56" s="59"/>
+      <c r="I56" s="59"/>
+      <c r="J56" s="60"/>
+      <c r="L56" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="M56" s="34"/>
-      <c r="N56" s="34"/>
-      <c r="O56" s="34"/>
-      <c r="P56" s="34"/>
-      <c r="Q56" s="34"/>
-      <c r="R56" s="34"/>
-      <c r="S56" s="34"/>
-      <c r="T56" s="35"/>
-      <c r="V56" s="33" t="s">
+      <c r="M56" s="59"/>
+      <c r="N56" s="59"/>
+      <c r="O56" s="59"/>
+      <c r="P56" s="59"/>
+      <c r="Q56" s="59"/>
+      <c r="R56" s="59"/>
+      <c r="S56" s="59"/>
+      <c r="T56" s="60"/>
+      <c r="V56" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="W56" s="34"/>
-      <c r="X56" s="34"/>
-      <c r="Y56" s="34"/>
-      <c r="Z56" s="34"/>
-      <c r="AA56" s="34"/>
-      <c r="AB56" s="34"/>
-      <c r="AC56" s="34"/>
-      <c r="AD56" s="34"/>
-      <c r="AE56" s="35"/>
+      <c r="W56" s="59"/>
+      <c r="X56" s="59"/>
+      <c r="Y56" s="59"/>
+      <c r="Z56" s="59"/>
+      <c r="AA56" s="59"/>
+      <c r="AB56" s="59"/>
+      <c r="AC56" s="59"/>
+      <c r="AD56" s="59"/>
+      <c r="AE56" s="60"/>
     </row>
     <row r="57" spans="1:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="12"/>
-      <c r="N57" s="42"/>
-      <c r="P57" s="30"/>
-      <c r="S57" s="42"/>
-      <c r="W57" s="28"/>
-      <c r="AA57" s="28"/>
-      <c r="AD57" s="31"/>
-    </row>
-    <row r="58" spans="1:31" s="87" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="98"/>
-      <c r="H58" s="88" t="s">
+      <c r="B57" s="5"/>
+      <c r="N57" s="20"/>
+      <c r="P57" s="14"/>
+      <c r="S57" s="20"/>
+      <c r="W57" s="12"/>
+      <c r="AA57" s="12"/>
+      <c r="AD57" s="15"/>
+    </row>
+    <row r="58" spans="1:31" s="50" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="52"/>
+      <c r="H58" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="I58" s="90"/>
-      <c r="J58" s="89"/>
-      <c r="L58" s="88" t="s">
+      <c r="I58" s="70"/>
+      <c r="J58" s="71"/>
+      <c r="L58" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="M58" s="90"/>
-      <c r="N58" s="89"/>
-      <c r="P58" s="97"/>
-      <c r="R58" s="88" t="s">
+      <c r="M58" s="70"/>
+      <c r="N58" s="71"/>
+      <c r="P58" s="51"/>
+      <c r="R58" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="S58" s="90"/>
-      <c r="T58" s="89"/>
-      <c r="V58" s="91" t="s">
+      <c r="S58" s="70"/>
+      <c r="T58" s="71"/>
+      <c r="V58" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="W58" s="92"/>
-      <c r="Y58" s="91" t="s">
+      <c r="W58" s="73"/>
+      <c r="Y58" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="Z58" s="95"/>
-      <c r="AA58" s="95"/>
-      <c r="AB58" s="92"/>
-      <c r="AD58" s="91" t="s">
+      <c r="Z58" s="76"/>
+      <c r="AA58" s="76"/>
+      <c r="AB58" s="73"/>
+      <c r="AD58" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="AE58" s="92"/>
-    </row>
-    <row r="59" spans="1:31" s="87" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="98"/>
-      <c r="F59" s="88" t="s">
+      <c r="AE58" s="73"/>
+    </row>
+    <row r="59" spans="1:31" s="50" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="52"/>
+      <c r="F59" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="G59" s="90"/>
-      <c r="H59" s="89"/>
-      <c r="O59" s="88" t="s">
+      <c r="G59" s="70"/>
+      <c r="H59" s="71"/>
+      <c r="O59" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="P59" s="90"/>
-      <c r="Q59" s="89"/>
-      <c r="V59" s="93"/>
-      <c r="W59" s="94"/>
-      <c r="Y59" s="93"/>
-      <c r="Z59" s="96"/>
-      <c r="AA59" s="96"/>
-      <c r="AB59" s="94"/>
-      <c r="AD59" s="93"/>
-      <c r="AE59" s="94"/>
-    </row>
-    <row r="60" spans="1:31" s="87" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="98"/>
-      <c r="E60" s="88" t="s">
+      <c r="P59" s="70"/>
+      <c r="Q59" s="71"/>
+      <c r="V59" s="74"/>
+      <c r="W59" s="75"/>
+      <c r="Y59" s="74"/>
+      <c r="Z59" s="77"/>
+      <c r="AA59" s="77"/>
+      <c r="AB59" s="75"/>
+      <c r="AD59" s="74"/>
+      <c r="AE59" s="75"/>
+    </row>
+    <row r="60" spans="1:31" s="50" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="52"/>
+      <c r="E60" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="F60" s="89"/>
-    </row>
-    <row r="61" spans="1:31" s="87" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="98"/>
-      <c r="D61" s="88" t="s">
+      <c r="F60" s="71"/>
+    </row>
+    <row r="61" spans="1:31" s="50" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="52"/>
+      <c r="D61" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="E61" s="89"/>
+      <c r="E61" s="71"/>
     </row>
     <row r="62" spans="1:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="12"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="12"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="33" t="s">
+      <c r="B63" s="5"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="34"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="34"/>
-      <c r="O63" s="34"/>
-      <c r="P63" s="34"/>
-      <c r="Q63" s="34"/>
-      <c r="R63" s="34"/>
-      <c r="S63" s="34"/>
-      <c r="T63" s="34"/>
-      <c r="U63" s="34"/>
-      <c r="V63" s="34"/>
-      <c r="W63" s="34"/>
-      <c r="X63" s="34"/>
-      <c r="Y63" s="34"/>
-      <c r="Z63" s="34"/>
-      <c r="AA63" s="34"/>
-      <c r="AB63" s="34"/>
-      <c r="AC63" s="34"/>
-      <c r="AD63" s="35"/>
+      <c r="F63" s="59"/>
+      <c r="G63" s="59"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="59"/>
+      <c r="J63" s="59"/>
+      <c r="K63" s="59"/>
+      <c r="L63" s="59"/>
+      <c r="M63" s="59"/>
+      <c r="N63" s="59"/>
+      <c r="O63" s="59"/>
+      <c r="P63" s="59"/>
+      <c r="Q63" s="59"/>
+      <c r="R63" s="59"/>
+      <c r="S63" s="59"/>
+      <c r="T63" s="59"/>
+      <c r="U63" s="59"/>
+      <c r="V63" s="59"/>
+      <c r="W63" s="59"/>
+      <c r="X63" s="59"/>
+      <c r="Y63" s="59"/>
+      <c r="Z63" s="59"/>
+      <c r="AA63" s="59"/>
+      <c r="AB63" s="59"/>
+      <c r="AC63" s="59"/>
+      <c r="AD63" s="60"/>
     </row>
     <row r="64" spans="1:31" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I64" s="28"/>
-      <c r="S64" s="28"/>
-      <c r="AA64" s="28"/>
+      <c r="I64" s="12"/>
+      <c r="S64" s="12"/>
+      <c r="AA64" s="12"/>
     </row>
     <row r="65" spans="4:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="33" t="s">
+      <c r="D65" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="34"/>
-      <c r="I65" s="34"/>
-      <c r="J65" s="34"/>
-      <c r="K65" s="34"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="86"/>
-      <c r="N65" s="33" t="s">
+      <c r="E65" s="59"/>
+      <c r="F65" s="59"/>
+      <c r="G65" s="59"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="59"/>
+      <c r="K65" s="59"/>
+      <c r="L65" s="60"/>
+      <c r="M65" s="49"/>
+      <c r="N65" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="O65" s="34"/>
-      <c r="P65" s="34"/>
-      <c r="Q65" s="34"/>
-      <c r="R65" s="34"/>
-      <c r="S65" s="34"/>
-      <c r="T65" s="34"/>
-      <c r="U65" s="34"/>
-      <c r="V65" s="35"/>
-      <c r="W65" s="86"/>
-      <c r="X65" s="33" t="s">
+      <c r="O65" s="59"/>
+      <c r="P65" s="59"/>
+      <c r="Q65" s="59"/>
+      <c r="R65" s="59"/>
+      <c r="S65" s="59"/>
+      <c r="T65" s="59"/>
+      <c r="U65" s="59"/>
+      <c r="V65" s="60"/>
+      <c r="W65" s="49"/>
+      <c r="X65" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="Y65" s="34"/>
-      <c r="Z65" s="34"/>
-      <c r="AA65" s="34"/>
-      <c r="AB65" s="34"/>
-      <c r="AC65" s="34"/>
-      <c r="AD65" s="34"/>
-      <c r="AE65" s="35"/>
+      <c r="Y65" s="59"/>
+      <c r="Z65" s="59"/>
+      <c r="AA65" s="59"/>
+      <c r="AB65" s="59"/>
+      <c r="AC65" s="59"/>
+      <c r="AD65" s="59"/>
+      <c r="AE65" s="60"/>
     </row>
     <row r="66" spans="4:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Y66" s="28"/>
-      <c r="AB66" s="28"/>
-      <c r="AD66" s="31"/>
+      <c r="Y66" s="12"/>
+      <c r="AB66" s="12"/>
+      <c r="AD66" s="15"/>
     </row>
     <row r="67" spans="4:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="101" t="s">
+      <c r="D67" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="E67" s="102"/>
-      <c r="H67" s="101" t="s">
+      <c r="E67" s="62"/>
+      <c r="H67" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I67" s="102"/>
-      <c r="K67" s="101" t="s">
+      <c r="I67" s="62"/>
+      <c r="K67" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="L67" s="102"/>
-      <c r="N67" s="101" t="s">
+      <c r="L67" s="62"/>
+      <c r="N67" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="O67" s="102"/>
-      <c r="R67" s="105" t="s">
+      <c r="O67" s="62"/>
+      <c r="R67" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="S67" s="106"/>
-      <c r="U67" s="101" t="s">
+      <c r="S67" s="66"/>
+      <c r="U67" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="V67" s="102"/>
-      <c r="X67" s="33" t="s">
+      <c r="V67" s="62"/>
+      <c r="X67" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="Y67" s="35"/>
-      <c r="AA67" s="33" t="s">
+      <c r="Y67" s="60"/>
+      <c r="AA67" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AB67" s="35"/>
-      <c r="AD67" s="33" t="s">
+      <c r="AB67" s="60"/>
+      <c r="AD67" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="AE67" s="35"/>
+      <c r="AE67" s="60"/>
     </row>
     <row r="68" spans="4:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="103"/>
-      <c r="E68" s="104"/>
-      <c r="H68" s="103"/>
-      <c r="I68" s="104"/>
-      <c r="K68" s="103"/>
-      <c r="L68" s="104"/>
-      <c r="N68" s="103"/>
-      <c r="O68" s="104"/>
-      <c r="R68" s="107"/>
-      <c r="S68" s="108"/>
-      <c r="U68" s="103"/>
-      <c r="V68" s="104"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="64"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="64"/>
+      <c r="K68" s="63"/>
+      <c r="L68" s="64"/>
+      <c r="N68" s="63"/>
+      <c r="O68" s="64"/>
+      <c r="R68" s="67"/>
+      <c r="S68" s="68"/>
+      <c r="U68" s="63"/>
+      <c r="V68" s="64"/>
     </row>
     <row r="69" spans="4:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z69" s="33" t="s">
+      <c r="Z69" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="AA69" s="34"/>
-      <c r="AB69" s="34"/>
-      <c r="AC69" s="34"/>
-      <c r="AD69" s="35"/>
+      <c r="AA69" s="59"/>
+      <c r="AB69" s="59"/>
+      <c r="AC69" s="59"/>
+      <c r="AD69" s="60"/>
     </row>
     <row r="70" spans="4:31" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P70" s="33" t="s">
+      <c r="P70" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="Q70" s="34"/>
-      <c r="R70" s="34"/>
-      <c r="S70" s="34"/>
-      <c r="T70" s="34"/>
-      <c r="U70" s="35"/>
-      <c r="Z70" s="33" t="s">
+      <c r="Q70" s="59"/>
+      <c r="R70" s="59"/>
+      <c r="S70" s="59"/>
+      <c r="T70" s="59"/>
+      <c r="U70" s="60"/>
+      <c r="Z70" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="AA70" s="34"/>
-      <c r="AB70" s="34"/>
-      <c r="AC70" s="34"/>
-      <c r="AD70" s="35"/>
+      <c r="AA70" s="59"/>
+      <c r="AB70" s="59"/>
+      <c r="AC70" s="59"/>
+      <c r="AD70" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="P70:U70"/>
-    <mergeCell ref="X67:Y67"/>
-    <mergeCell ref="AA67:AB67"/>
-    <mergeCell ref="AD67:AE67"/>
-    <mergeCell ref="Z69:AD69"/>
-    <mergeCell ref="Z70:AD70"/>
-    <mergeCell ref="D67:E68"/>
-    <mergeCell ref="H67:I68"/>
-    <mergeCell ref="K67:L68"/>
-    <mergeCell ref="N67:O68"/>
-    <mergeCell ref="R67:S68"/>
-    <mergeCell ref="U67:V68"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="X7:AD7"/>
+    <mergeCell ref="O11:U11"/>
+    <mergeCell ref="O3:U3"/>
+    <mergeCell ref="X3:AD3"/>
+    <mergeCell ref="X11:AD11"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="E16:N16"/>
+    <mergeCell ref="R16:X16"/>
+    <mergeCell ref="O7:U7"/>
+    <mergeCell ref="AA35:AD35"/>
+    <mergeCell ref="AB37:AD37"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="R41:W41"/>
+    <mergeCell ref="R28:W28"/>
+    <mergeCell ref="AB39:AD39"/>
+    <mergeCell ref="AB41:AD41"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="U39:W39"/>
+    <mergeCell ref="U43:W43"/>
+    <mergeCell ref="U45:W45"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="Z18:AE18"/>
+    <mergeCell ref="AA28:AD28"/>
+    <mergeCell ref="AA31:AD31"/>
+    <mergeCell ref="AA33:AD33"/>
+    <mergeCell ref="AA20:AD20"/>
+    <mergeCell ref="AA22:AD22"/>
+    <mergeCell ref="AA24:AD24"/>
+    <mergeCell ref="AA26:AD26"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="U33:W33"/>
+    <mergeCell ref="R20:U20"/>
+    <mergeCell ref="R24:U24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="AB43:AD43"/>
+    <mergeCell ref="AB45:AD45"/>
+    <mergeCell ref="AB47:AD47"/>
+    <mergeCell ref="AB49:AD49"/>
+    <mergeCell ref="AB51:AD51"/>
+    <mergeCell ref="O59:Q59"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="E54:W54"/>
+    <mergeCell ref="U47:W47"/>
+    <mergeCell ref="U49:W49"/>
+    <mergeCell ref="U35:W35"/>
+    <mergeCell ref="U37:W37"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="N28:O28"/>
     <mergeCell ref="L56:T56"/>
     <mergeCell ref="E63:AD63"/>
     <mergeCell ref="X65:AE65"/>
@@ -4024,71 +4085,18 @@
     <mergeCell ref="E60:F60"/>
     <mergeCell ref="H58:J58"/>
     <mergeCell ref="L58:N58"/>
-    <mergeCell ref="O59:Q59"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="E54:W54"/>
-    <mergeCell ref="AB43:AD43"/>
-    <mergeCell ref="AB45:AD45"/>
-    <mergeCell ref="AB47:AD47"/>
-    <mergeCell ref="AB49:AD49"/>
-    <mergeCell ref="AB51:AD51"/>
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="Z18:AE18"/>
-    <mergeCell ref="AA28:AD28"/>
-    <mergeCell ref="AA31:AD31"/>
-    <mergeCell ref="AA33:AD33"/>
-    <mergeCell ref="AA35:AD35"/>
-    <mergeCell ref="AB37:AD37"/>
-    <mergeCell ref="N51:O51"/>
-    <mergeCell ref="R41:W41"/>
-    <mergeCell ref="R28:W28"/>
-    <mergeCell ref="AA20:AD20"/>
-    <mergeCell ref="AA22:AD22"/>
-    <mergeCell ref="AA24:AD24"/>
-    <mergeCell ref="AA26:AD26"/>
-    <mergeCell ref="AB39:AD39"/>
-    <mergeCell ref="AB41:AD41"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="U39:W39"/>
-    <mergeCell ref="U43:W43"/>
-    <mergeCell ref="U45:W45"/>
-    <mergeCell ref="U47:W47"/>
-    <mergeCell ref="U49:W49"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="U33:W33"/>
-    <mergeCell ref="U35:W35"/>
-    <mergeCell ref="U37:W37"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="R20:U20"/>
-    <mergeCell ref="R24:U24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="X11:AD11"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="E16:N16"/>
-    <mergeCell ref="R16:X16"/>
-    <mergeCell ref="O7:U7"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="X7:AD7"/>
-    <mergeCell ref="O11:U11"/>
-    <mergeCell ref="O3:U3"/>
-    <mergeCell ref="X3:AD3"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="D67:E68"/>
+    <mergeCell ref="H67:I68"/>
+    <mergeCell ref="K67:L68"/>
+    <mergeCell ref="N67:O68"/>
+    <mergeCell ref="R67:S68"/>
+    <mergeCell ref="P70:U70"/>
+    <mergeCell ref="X67:Y67"/>
+    <mergeCell ref="AA67:AB67"/>
+    <mergeCell ref="AD67:AE67"/>
+    <mergeCell ref="Z69:AD69"/>
+    <mergeCell ref="Z70:AD70"/>
+    <mergeCell ref="U67:V68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="48" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4099,8 +4107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09C75FA-2A7E-46EF-937C-958B69EE8756}">
   <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4112,7 +4120,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="57" t="s">
         <v>177</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -4120,7 +4128,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="57" t="s">
         <v>178</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -4128,7 +4136,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="57" t="s">
         <v>179</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -4136,7 +4144,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="57" t="s">
         <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -4150,7 +4158,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="57" t="s">
         <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -4158,7 +4166,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="57" t="s">
         <v>182</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -4166,7 +4174,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="57" t="s">
         <v>183</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -4174,7 +4182,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="57" t="s">
         <v>184</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -4182,7 +4190,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="57" t="s">
         <v>185</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -4190,7 +4198,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="57" t="s">
         <v>186</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -4198,7 +4206,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="57" t="s">
         <v>187</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -4206,7 +4214,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="57" t="s">
         <v>188</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -4214,7 +4222,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="57" t="s">
         <v>189</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -4222,7 +4230,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="57" t="s">
         <v>190</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -4230,27 +4238,27 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="111" t="s">
+      <c r="B16" s="57" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="111" t="s">
+      <c r="B17" s="57" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="111" t="s">
+      <c r="B18" s="57" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="111" t="s">
+      <c r="B19" s="57" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="57" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4278,142 +4286,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="2" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85" t="s">
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109" t="s">
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
     </row>
     <row r="8" spans="2:5" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="110" t="s">
+      <c r="B8" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="110" t="s">
+      <c r="C8" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110" t="s">
+      <c r="D8" s="56"/>
+      <c r="E8" s="56" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85" t="s">
+      <c r="D11" s="48"/>
+      <c r="E11" s="48" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85" t="s">
+      <c r="D12" s="48"/>
+      <c r="E12" s="48" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="85"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
     </row>
     <row r="14" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
     </row>
     <row r="15" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="85"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
     </row>
     <row r="16" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
     </row>
     <row r="17" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -4421,48 +4429,48 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="85" t="s">
+      <c r="C22" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85" t="s">
+      <c r="D22" s="48"/>
+      <c r="E22" s="48" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
     </row>
     <row r="24" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="85"/>
-      <c r="C24" s="85" t="s">
+      <c r="B24" s="48"/>
+      <c r="C24" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="85"/>
-      <c r="E24" s="85"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
     </row>
     <row r="25" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
     </row>
     <row r="26" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="85"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
     </row>
     <row r="27" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="85"/>
-      <c r="C27" s="85"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4473,11 +4481,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36928A4B-4C56-48AB-B2A6-14873B9DEC7E}">
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>